<commit_message>
More work on IoT, including support in HTTP Request.lvclass for 'PATCH' HTTP Verb.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - IoT.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - IoT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Code</t>
   </si>
@@ -36,6 +36,67 @@
   </si>
   <si>
     <t>You cannot specify more than 3 attributes when creating a Thing.</t>
+  </si>
+  <si>
+    <t>InternalFailureException - An unexpected error has occurred.</t>
+  </si>
+  <si>
+    <t>InvalidRequestException - The request is not valid.</t>
+  </si>
+  <si>
+    <t>ResourceNotFoundException - The specified resource does not exist.</t>
+  </si>
+  <si>
+    <t>ServiceUnavailableException - The service is temporarily unavailable.</t>
+  </si>
+  <si>
+    <t>ThrottlingException - The rate exceeds the limit.</t>
+  </si>
+  <si>
+    <t>TransferAlreadyCompletedException - You can't revert the certificate transfer because the transfer is already complete.</t>
+  </si>
+  <si>
+    <t>UnauthorizedException - You are not authorized to perform this operation.</t>
+  </si>
+  <si>
+    <t>LimitExceededException - The number of attached entities exceeds the limit.</t>
+  </si>
+  <si>
+    <t>MalformedPolicyException - The policy documentation is not valid.</t>
+  </si>
+  <si>
+    <t>ResourceAlreadyExistsException - The resource already exists.</t>
+  </si>
+  <si>
+    <t>VersionsLimitExceededException - The number of policy versions exceeds the limit.</t>
+  </si>
+  <si>
+    <t>InternalException - An unexpected error has occurred.</t>
+  </si>
+  <si>
+    <t>SqlParseException - The Rule-SQL expression cannot be parsed correctly.</t>
+  </si>
+  <si>
+    <t>CertificateStateException - The certificate operation is not allowed.</t>
+  </si>
+  <si>
+    <t>DeleteConflictException - You cannot delete the resource because it is attached to one or more resources.</t>
+  </si>
+  <si>
+    <t>VersionConflictException - The version of the thing is different than the version specified with the --version parameter.</t>
+  </si>
+  <si>
+    <t>CertificateValidationException - The certificate is invalid.</t>
+  </si>
+  <si>
+    <t>RegistrationCodeValidationException - The registration code is invalid.</t>
+  </si>
+  <si>
+    <t>CertificateConflictException - Unable to verify the CA certificate used to sign the device certificate you are attempting to register. This happens when you have registered 
+more than one CA certificate that has the same subject field and public key.</t>
+  </si>
+  <si>
+    <t>TransferConflictException - You cannot transfer the certificate because authorization policies are still attached.</t>
   </si>
 </sst>
 </file>
@@ -408,7 +469,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +502,166 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>412402</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>412403</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>412404</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>412405</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>412406</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>412407</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>412408</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>412409</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>412410</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>412411</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>412412</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>412413</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>412414</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>412415</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>412416</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>412417</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>412418</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>412419</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>412420</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>412421</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added several new IoT methods.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - IoT.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - IoT.xlsx
@@ -32,9 +32,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>The Thing name cannot be blank.</t>
-  </si>
-  <si>
     <t>You cannot specify more than 3 attributes when creating a Thing.</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>TransferConflictException - You cannot transfer the certificate because authorization policies are still attached.</t>
+  </si>
+  <si>
+    <t>A required string field was blank.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>412400</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>412401</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>412402</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -515,7 +515,7 @@
         <v>412403</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>412404</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>412405</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
         <v>412406</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>412407</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>412408</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>412409</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>412410</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>412411</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>412412</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>412413</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
         <v>412414</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>412415</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>412416</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>412417</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>412418</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>412419</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>412420</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>412421</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished all 'green' IoT methods and several 'yellow' ones as well.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - IoT.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - IoT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Code</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>A required string field was blank.</t>
+  </si>
+  <si>
+    <t>NotFoundException - The specified resource does not exist.</t>
+  </si>
+  <si>
+    <t>You must specify a version number greater than 0.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,6 +668,22 @@
         <v>22</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>412422</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>412423</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>

</xml_diff>